<commit_message>
first updates for all realm
</commit_message>
<xml_diff>
--- a/cmip6/models/mri-esm2-0/cmip6_mri_mri-esm2-0_ocnbgchem.xlsx
+++ b/cmip6/models/mri-esm2-0/cmip6_mri_mri-esm2-0_ocnbgchem.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yukimoto/Documents/研究計画・プロジェクト/CMIP6/Documentation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD5B984-448C-5A4A-9D54-26349934C022}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="19940" yWindow="460" windowWidth="24560" windowHeight="23680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,12 @@
     <sheet name="1. Key Properties" sheetId="3" r:id="rId3"/>
     <sheet name="2. Tracers" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="436">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -142,9 +148,6 @@
     <t>cmip6.ocnbgchem.key_properties.name</t>
   </si>
   <si>
-    <t>Ocean Biogeo Chemistry (MRI.COM3)</t>
-  </si>
-  <si>
     <t>1.1.1.2 *</t>
   </si>
   <si>
@@ -247,9 +250,6 @@
     <t>cmip6.ocnbgchem.key_properties.prognostic_variables</t>
   </si>
   <si>
-    <t>Nitrate, Phosphate, Phytoplankton, Zooplankton, Detritus, Total CO2, Alkalinity, Oxygen</t>
-  </si>
-  <si>
     <t>1.1.1.8 *</t>
   </si>
   <si>
@@ -502,9 +502,6 @@
     <t>cmip6.ocnbgchem.key_properties.gas_exchange.CO2_exchange_type</t>
   </si>
   <si>
-    <t>Other: wanninkhof</t>
-  </si>
-  <si>
     <t>OMIP protocol</t>
   </si>
   <si>
@@ -1120,9 +1117,6 @@
     <t>cmip6.ocnbgchem.tracers.disolved_organic_matter.lability</t>
   </si>
   <si>
-    <t>Other: no</t>
-  </si>
-  <si>
     <t>Labile</t>
   </si>
   <si>
@@ -1292,17 +1286,76 @@
   </si>
   <si>
     <t>Diagnostic)</t>
+  </si>
+  <si>
+    <t>MRI.COM ver. 4.4</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>OMIP protocol</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>CFC-11, CFC-12, SF6, Dissolved inorganic carbon, Natural dissolved inorganic carbon, Abiotic dissolved inorganic carbon, Abiotic dissolved inorganic 14carbon, Total alkalinity, Dissolved oxygen, Phosphate, Nitrate, Phytoplankton, Zooplankton, Detritus</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>NPZD, no Fe.</t>
+  </si>
+  <si>
+    <t>C, N, O2, P</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Carbonate Ion</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Primary production</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Surface nitrate concentration in the HNLC regions</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>No upper trophic level model is included.</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>The advection scheme for the ocean biogeochemistry tracers is the Multidimensional Positive Definite Advection Transport Algorithm (MPDATA; Smolarkiewicz and Margolin, 1998) scheme.</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t xml:space="preserve">A simple NPZD model is used for biology. Iron is not included. Dissolved inorganic carbon (DIC), total alkalinity, and dissolved oxygen (DO) are changed by the nutrient change in the NPZD model assuming the Redfield ratio P:N:C:O2 = 1:16:106:-138. DIC and DO are also changed by the surface flux. The model does not include any nutrient input from river, atmosphere and ocean floor. </t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Some parameters in NPZD model are tuned so that following targets get reasonable values. They are overall surface Chlorophyll-a concentration pattern, gross primary production, surface nitrarate concentration in high-nutrient low-cholorophyll (HNLC) region in the North Pacific and the Southern Ocean. This tuning may deteriorate nutrient trapping in the eastern Equator.</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>MRI</t>
+    <phoneticPr fontId="15"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1399,6 +1452,13 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1490,15 +1550,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1540,7 +1608,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1572,9 +1640,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1606,6 +1692,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1781,24 +1885,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="180.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="20">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1806,7 +1910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="20">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1814,7 +1918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="20">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1822,7 +1926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="20">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1830,7 +1934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="20">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1838,12 +1942,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="20">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="18">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1851,7 +1955,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="18">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1859,7 +1963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="18">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1867,7 +1971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="18">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1875,41 +1979,44 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="20">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="20">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="15"/>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1"/>
-    <hyperlink ref="B12" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="80.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -1920,7 +2027,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="18">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
@@ -1944,11 +2051,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="11"/>
+    <row r="9" spans="1:2" ht="19">
+      <c r="A9" s="11" t="s">
+        <v>435</v>
+      </c>
       <c r="B9" s="11"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="18">
       <c r="A12" s="9" t="s">
         <v>29</v>
       </c>
@@ -1972,39 +2081,42 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="18">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="15"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Top Level,Key Properties,Tracers"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-    <hyperlink ref="A13" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD235"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AD235"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="B235" sqref="B235"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -2041,15 +2153,15 @@
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
       <c r="B6" s="11" t="s">
-        <v>41</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -2057,26 +2169,28 @@
         <v>38</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -2084,91 +2198,97 @@
         <v>38</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="178" customHeight="1">
-      <c r="B16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="18" spans="1:30" ht="24" customHeight="1">
       <c r="A18" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="24" customHeight="1">
       <c r="A19" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="C19" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="10" t="s">
+    </row>
+    <row r="20" spans="1:30" ht="24" customHeight="1">
+      <c r="B20" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA20" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:30" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
-      <c r="AA20" s="6" t="s">
+      <c r="AB20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="AB20" s="6" t="s">
+      <c r="AC20" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AC20" s="6" t="s">
+      <c r="AD20" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="AD20" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="24" customHeight="1">
       <c r="A22" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:30" ht="24" customHeight="1">
       <c r="A23" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="10" t="s">
+    </row>
+    <row r="24" spans="1:30" ht="24" customHeight="1">
+      <c r="B24" s="11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="1:30" ht="24" customHeight="1">
-      <c r="B24" s="11"/>
       <c r="AA24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB24" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AB24" s="6" t="s">
+      <c r="AC24" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="AC24" s="6" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="24" customHeight="1">
       <c r="A26" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:30" ht="24" customHeight="1">
@@ -2176,26 +2296,28 @@
         <v>38</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:30" ht="24" customHeight="1">
       <c r="B28" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="24" customHeight="1">
-      <c r="B29" s="11"/>
+      <c r="B29" s="11" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="31" spans="1:30" ht="24" customHeight="1">
       <c r="A31" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:30" ht="24" customHeight="1">
@@ -2203,28 +2325,28 @@
         <v>38</v>
       </c>
       <c r="B32" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
       <c r="B33" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="38" customHeight="1">
       <c r="B34" s="11" t="s">
-        <v>76</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="24" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
@@ -2232,26 +2354,28 @@
         <v>38</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" customHeight="1">
       <c r="B38" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
-      <c r="B39" s="11"/>
+      <c r="B39" s="11" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1">
       <c r="A41" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="24" customHeight="1">
@@ -2259,75 +2383,77 @@
         <v>38</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
-      <c r="B43" s="11"/>
+      <c r="B43" s="11" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="46" spans="1:3" ht="24" customHeight="1">
       <c r="A46" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="24" customHeight="1">
       <c r="B47" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:28" ht="24" customHeight="1">
       <c r="A49" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:28" ht="24" customHeight="1">
       <c r="A50" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:28" ht="24" customHeight="1">
       <c r="B51" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA51" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AB51" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:28" ht="24" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:28" ht="24" customHeight="1">
       <c r="A54" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:28" ht="24" customHeight="1">
@@ -2335,62 +2461,64 @@
     </row>
     <row r="58" spans="1:28" ht="24" customHeight="1">
       <c r="A58" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:28" ht="24" customHeight="1">
       <c r="B59" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:28" ht="24" customHeight="1">
       <c r="A61" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="1:28" ht="24" customHeight="1">
       <c r="A62" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:28" ht="24" customHeight="1">
-      <c r="B63" s="11"/>
+      <c r="B63" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="AA63" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AB63" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:28" ht="24" customHeight="1">
       <c r="A65" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:28" ht="24" customHeight="1">
       <c r="A66" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:28" ht="24" customHeight="1">
@@ -2398,79 +2526,83 @@
     </row>
     <row r="70" spans="1:28" ht="24" customHeight="1">
       <c r="A70" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:28" ht="24" customHeight="1">
       <c r="B71" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:28" ht="24" customHeight="1">
       <c r="A73" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:28" ht="24" customHeight="1">
       <c r="A74" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B74" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" ht="24" customHeight="1">
+      <c r="B75" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA75" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="AB75" s="6" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="75" spans="1:28" ht="24" customHeight="1">
-      <c r="B75" s="11"/>
-      <c r="AA75" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="AB75" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:28" ht="24" customHeight="1">
       <c r="A77" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="1:28" ht="24" customHeight="1">
       <c r="A78" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B78" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" ht="24" customHeight="1">
+      <c r="B79" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C78" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="79" spans="1:28" ht="24" customHeight="1">
-      <c r="B79" s="11"/>
       <c r="AA79" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AB79" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="1:29" ht="24" customHeight="1">
       <c r="A81" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:29" ht="24" customHeight="1">
@@ -2478,101 +2610,107 @@
         <v>38</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="83" spans="1:29" ht="24" customHeight="1">
       <c r="B83" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:29" ht="178" customHeight="1">
-      <c r="B84" s="11"/>
+      <c r="B84" s="11" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="87" spans="1:29" ht="24" customHeight="1">
       <c r="A87" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88" spans="1:29" ht="24" customHeight="1">
       <c r="B88" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="1:29" ht="24" customHeight="1">
       <c r="A90" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:29" ht="24" customHeight="1">
       <c r="A91" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B91" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29" ht="24" customHeight="1">
+      <c r="B92" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA92" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="AB92" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="92" spans="1:29" ht="24" customHeight="1">
-      <c r="B92" s="11"/>
-      <c r="AA92" s="6" t="s">
+      <c r="AC92" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="AB92" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC92" s="6" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="94" spans="1:29" ht="24" customHeight="1">
       <c r="A94" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:29" ht="24" customHeight="1">
       <c r="A95" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B95" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29" ht="24" customHeight="1">
+      <c r="B96" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C95" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="96" spans="1:29" ht="24" customHeight="1">
-      <c r="B96" s="11"/>
       <c r="AA96" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AB96" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AC96" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="24" customHeight="1">
       <c r="A98" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="24" customHeight="1">
@@ -2580,26 +2718,28 @@
         <v>38</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="24" customHeight="1">
       <c r="B100" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="24" customHeight="1">
-      <c r="B101" s="11"/>
+      <c r="B101" s="11" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="103" spans="1:3" ht="24" customHeight="1">
       <c r="A103" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="24" customHeight="1">
@@ -2607,50 +2747,52 @@
         <v>38</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1">
       <c r="B105" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="24" customHeight="1">
-      <c r="B106" s="11"/>
+      <c r="B106" s="11" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="109" spans="1:3" ht="24" customHeight="1">
       <c r="A109" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="24" customHeight="1">
       <c r="B110" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="24" customHeight="1">
       <c r="A112" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="113" spans="1:28" ht="24" customHeight="1">
       <c r="A113" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B113" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C113" s="10" t="s">
         <v>154</v>
-      </c>
-      <c r="B113" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C113" s="10" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="114" spans="1:28" ht="24" customHeight="1">
@@ -2660,51 +2802,51 @@
     </row>
     <row r="116" spans="1:28" ht="24" customHeight="1">
       <c r="A116" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="117" spans="1:28" ht="24" customHeight="1">
       <c r="A117" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="118" spans="1:28" ht="24" customHeight="1">
       <c r="B118" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AA118" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AB118" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="120" spans="1:28" ht="24" customHeight="1">
       <c r="A120" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="121" spans="1:28" ht="24" customHeight="1">
       <c r="A121" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="122" spans="1:28" ht="24" customHeight="1">
@@ -2714,64 +2856,64 @@
     </row>
     <row r="124" spans="1:28" ht="24" customHeight="1">
       <c r="A124" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="125" spans="1:28" ht="24" customHeight="1">
       <c r="A125" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B125" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C125" s="10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="126" spans="1:28" ht="24" customHeight="1">
       <c r="B126" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AA126" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AB126" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="128" spans="1:28" ht="24" customHeight="1">
       <c r="A128" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="24" customHeight="1">
       <c r="A129" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B129" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C129" s="10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="24" customHeight="1">
       <c r="B130" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="24" customHeight="1">
       <c r="A132" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="24" customHeight="1">
@@ -2779,45 +2921,47 @@
         <v>38</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C133" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="24" customHeight="1">
-      <c r="B134" s="11"/>
+      <c r="B134" s="11" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="136" spans="1:3" ht="24" customHeight="1">
       <c r="A136" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="24" customHeight="1">
       <c r="A137" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="24" customHeight="1">
       <c r="B138" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="24" customHeight="1">
       <c r="A140" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="24" customHeight="1">
@@ -2825,45 +2969,47 @@
         <v>38</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="24" customHeight="1">
-      <c r="B142" s="11"/>
+      <c r="B142" s="11" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="144" spans="1:3" ht="24" customHeight="1">
       <c r="A144" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="24" customHeight="1">
       <c r="A145" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="24" customHeight="1">
       <c r="B146" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="24" customHeight="1">
       <c r="A148" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="24" customHeight="1">
@@ -2871,43 +3017,47 @@
         <v>38</v>
       </c>
       <c r="B149" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C149" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="24" customHeight="1">
-      <c r="B150" s="11"/>
+      <c r="B150" s="11" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="152" spans="1:3" ht="24" customHeight="1">
       <c r="A152" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="24" customHeight="1">
       <c r="A153" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="24" customHeight="1">
-      <c r="B154" s="11"/>
+      <c r="B154" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="156" spans="1:3" ht="24" customHeight="1">
       <c r="A156" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="24" customHeight="1">
@@ -2915,43 +3065,47 @@
         <v>38</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="24" customHeight="1">
-      <c r="B158" s="11"/>
+      <c r="B158" s="11" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="160" spans="1:3" ht="24" customHeight="1">
       <c r="A160" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="24" customHeight="1">
       <c r="A161" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B161" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C161" s="10" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="24" customHeight="1">
-      <c r="B162" s="11"/>
+      <c r="B162" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="164" spans="1:3" ht="24" customHeight="1">
       <c r="A164" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="24" customHeight="1">
@@ -2959,43 +3113,47 @@
         <v>38</v>
       </c>
       <c r="B165" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C165" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="24" customHeight="1">
-      <c r="B166" s="11"/>
+      <c r="B166" s="11" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="168" spans="1:3" ht="24" customHeight="1">
       <c r="A168" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="24" customHeight="1">
       <c r="A169" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B169" s="10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="24" customHeight="1">
-      <c r="B170" s="11"/>
+      <c r="B170" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="172" spans="1:3" ht="24" customHeight="1">
       <c r="A172" s="9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="24" customHeight="1">
@@ -3003,43 +3161,47 @@
         <v>38</v>
       </c>
       <c r="B173" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C173" s="10" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="24" customHeight="1">
-      <c r="B174" s="11"/>
+      <c r="B174" s="11" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="176" spans="1:3" ht="24" customHeight="1">
       <c r="A176" s="9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="24" customHeight="1">
       <c r="A177" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B177" s="10" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C177" s="10" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="24" customHeight="1">
-      <c r="B178" s="11"/>
+      <c r="B178" s="11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="180" spans="1:3" ht="24" customHeight="1">
       <c r="A180" s="9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="24" customHeight="1">
@@ -3047,43 +3209,47 @@
         <v>38</v>
       </c>
       <c r="B181" s="10" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="24" customHeight="1">
-      <c r="B182" s="11"/>
+      <c r="B182" s="11" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="184" spans="1:3" ht="24" customHeight="1">
       <c r="A184" s="9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="24" customHeight="1">
       <c r="A185" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B185" s="10" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C185" s="10" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="24" customHeight="1">
-      <c r="B186" s="11"/>
+      <c r="B186" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="188" spans="1:3" ht="24" customHeight="1">
       <c r="A188" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="24" customHeight="1">
@@ -3091,21 +3257,23 @@
         <v>38</v>
       </c>
       <c r="B189" s="10" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="24" customHeight="1">
-      <c r="B190" s="11"/>
+      <c r="B190" s="11" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="192" spans="1:3" ht="24" customHeight="1">
       <c r="A192" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="193" spans="1:29" ht="24" customHeight="1">
@@ -3113,95 +3281,97 @@
         <v>38</v>
       </c>
       <c r="B193" s="10" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="194" spans="1:29" ht="24" customHeight="1">
-      <c r="B194" s="11"/>
+      <c r="B194" s="11" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="197" spans="1:29" ht="24" customHeight="1">
       <c r="A197" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B197" s="12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="198" spans="1:29" ht="24" customHeight="1">
       <c r="B198" s="13" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="200" spans="1:29" ht="24" customHeight="1">
       <c r="A200" s="9" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="201" spans="1:29" ht="24" customHeight="1">
       <c r="A201" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B201" s="10" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C201" s="10" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="202" spans="1:29" ht="24" customHeight="1">
-      <c r="B202" s="11"/>
+      <c r="B202" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="AA202" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AB202" s="6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="204" spans="1:29" ht="24" customHeight="1">
       <c r="A204" s="9" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="205" spans="1:29" ht="24" customHeight="1">
       <c r="A205" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B205" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C205" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="206" spans="1:29" ht="24" customHeight="1">
+      <c r="B206" s="11"/>
+      <c r="AA206" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AB206" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="C205" s="10" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="206" spans="1:29" ht="24" customHeight="1">
-      <c r="B206" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="AA206" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="AB206" s="6" t="s">
-        <v>251</v>
-      </c>
       <c r="AC206" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="208" spans="1:29" ht="24" customHeight="1">
       <c r="A208" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="24" customHeight="1">
@@ -3209,15 +3379,15 @@
         <v>38</v>
       </c>
       <c r="B209" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C209" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="24" customHeight="1">
       <c r="B210" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="24" customHeight="1">
@@ -3225,23 +3395,23 @@
     </row>
     <row r="214" spans="1:3" ht="24" customHeight="1">
       <c r="A214" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B214" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="24" customHeight="1">
       <c r="B215" s="13" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="24" customHeight="1">
       <c r="A217" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B217" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="24" customHeight="1">
@@ -3249,26 +3419,28 @@
         <v>38</v>
       </c>
       <c r="B218" s="10" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C218" s="10" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="24" customHeight="1">
       <c r="B219" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="178" customHeight="1">
-      <c r="B220" s="11"/>
+      <c r="B220" s="11" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="222" spans="1:3" ht="24" customHeight="1">
       <c r="A222" s="9" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B222" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="24" customHeight="1">
@@ -3276,26 +3448,28 @@
         <v>38</v>
       </c>
       <c r="B223" s="10" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C223" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="24" customHeight="1">
       <c r="B224" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="24" customHeight="1">
-      <c r="B225" s="11"/>
+      <c r="B225" s="11" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="227" spans="1:3" ht="24" customHeight="1">
       <c r="A227" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B227" s="9" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="24" customHeight="1">
@@ -3303,26 +3477,28 @@
         <v>38</v>
       </c>
       <c r="B228" s="10" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C228" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="24" customHeight="1">
       <c r="B229" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="24" customHeight="1">
-      <c r="B230" s="11"/>
+      <c r="B230" s="11" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="232" spans="1:3" ht="24" customHeight="1">
       <c r="A232" s="9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B232" s="9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="24" customHeight="1">
@@ -3330,93 +3506,37 @@
         <v>38</v>
       </c>
       <c r="B233" s="10" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C233" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="24" customHeight="1">
       <c r="B234" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="235" spans="1:3" ht="24" customHeight="1">
       <c r="B235" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="24">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>AA20:AD20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24 B206 B96 B92" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>AA24:AC24</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51 B202 B126 B118 B79 B75 B63" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>AA51:AB51</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55 B67" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63">
-      <formula1>AA63:AB63</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B67">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
-      <formula1>AA75:AB75</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79">
-      <formula1>AA79:AB79</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92">
-      <formula1>AA92:AC92</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B96">
-      <formula1>AA96:AC96</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B114">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B114 B186 B178 B170 B162 B154 B146 B138 B130 B122" xr:uid="{00000000-0002-0000-0200-00000A000000}">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B118">
-      <formula1>AA118:AB118</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B122">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B126">
-      <formula1>AA126:AB126</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B130">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B138">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B146">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B154">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B162">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B170">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B178">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B186">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B202">
-      <formula1>AA202:AB202</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B206">
-      <formula1>AA206:AC206</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3424,35 +3544,37 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD128"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AE130"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B130" sqref="B130"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>37</v>
@@ -3463,10 +3585,10 @@
         <v>38</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
@@ -3474,10 +3596,10 @@
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -3485,15 +3607,15 @@
         <v>38</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="178" customHeight="1">
@@ -3501,45 +3623,45 @@
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:31" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="24" customHeight="1">
       <c r="A18" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="24" customHeight="1">
@@ -3548,780 +3670,801 @@
       </c>
     </row>
     <row r="20" spans="1:31" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>289</v>
+      </c>
       <c r="AA20" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="AB20" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="AC20" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="AD20" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="AB20" s="6" t="s">
+      <c r="AE20" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" ht="24" customHeight="1">
+      <c r="B21" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="AA21" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="AB21" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="AC21" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="AE21" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" ht="24" customHeight="1">
+      <c r="A23" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="AC20" s="6" t="s">
+      <c r="B23" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="AD20" s="6" t="s">
+    </row>
+    <row r="24" spans="1:31" ht="24" customHeight="1">
+      <c r="A24" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="AE20" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" ht="24" customHeight="1">
-      <c r="A22" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="B22" s="9" t="s">
+    </row>
+    <row r="25" spans="1:31" ht="24" customHeight="1">
+      <c r="B25" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" ht="24" customHeight="1">
+      <c r="B26" s="11" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="23" spans="1:31" ht="24" customHeight="1">
-      <c r="A23" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="10" t="s">
+      <c r="AA26" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="AB26" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="AC26" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" ht="24" customHeight="1">
+      <c r="A28" s="9" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="24" spans="1:31" ht="24" customHeight="1">
-      <c r="B24" s="10" t="s">
+      <c r="B28" s="9" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" ht="24" customHeight="1">
+      <c r="A29" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" ht="24" customHeight="1">
+      <c r="B30" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="24" customHeight="1">
-      <c r="B25" s="11"/>
-      <c r="AA25" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="AB25" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="AC25" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" ht="24" customHeight="1">
-      <c r="A27" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="B27" s="9" t="s">
+    <row r="31" spans="1:31" ht="24" customHeight="1">
+      <c r="B31" s="11"/>
+      <c r="AA31" s="6" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="28" spans="1:31" ht="24" customHeight="1">
-      <c r="A28" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="10" t="s">
+      <c r="AB31" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="AC31" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="24" customHeight="1">
+      <c r="A34" s="12" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="29" spans="1:31" ht="24" customHeight="1">
-      <c r="B29" s="10" t="s">
+      <c r="B34" s="12" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="24" customHeight="1">
+      <c r="B35" s="13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="24" customHeight="1">
+      <c r="A37" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="24" customHeight="1">
+      <c r="A38" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="24" customHeight="1">
+      <c r="B39" s="11" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="24" customHeight="1">
+      <c r="A41" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="24" customHeight="1">
+      <c r="A42" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="24" customHeight="1">
+      <c r="B43" s="11" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="24" customHeight="1">
+      <c r="A46" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="24" customHeight="1">
+      <c r="B47" s="13" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" ht="24" customHeight="1">
+      <c r="A49" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" ht="24" customHeight="1">
+      <c r="A50" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31" ht="24" customHeight="1">
+      <c r="B51" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="AA51" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="AB51" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="AC51" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="AD51" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="AE51" s="6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31" ht="24" customHeight="1">
+      <c r="A53" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" ht="24" customHeight="1">
+      <c r="A54" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31" ht="24" customHeight="1">
+      <c r="B55" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="24" customHeight="1">
-      <c r="B30" s="11"/>
-      <c r="AA30" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="AB30" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="AC30" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="24" customHeight="1">
-      <c r="A33" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1">
-      <c r="B34" s="13" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="24" customHeight="1">
-      <c r="A36" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="24" customHeight="1">
-      <c r="A37" s="14" t="s">
+    <row r="56" spans="1:31" ht="24" customHeight="1">
+      <c r="B56" s="11"/>
+      <c r="AA56" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="AB56" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="AC56" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="AD56" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" ht="24" customHeight="1">
+      <c r="A58" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31" ht="24" customHeight="1">
+      <c r="A59" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31" ht="24" customHeight="1">
+      <c r="B60" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31" ht="24" customHeight="1">
+      <c r="B61" s="11"/>
+      <c r="AA61" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="AB61" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC61" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="AD61" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31" ht="24" customHeight="1">
+      <c r="A64" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="65" spans="1:30" ht="24" customHeight="1">
+      <c r="B65" s="13" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="67" spans="1:30" ht="24" customHeight="1">
+      <c r="A67" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:30" ht="24" customHeight="1">
+      <c r="A68" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30" ht="24" customHeight="1">
+      <c r="B69" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="AA69" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="AB69" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="AC69" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="AD69" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" ht="24" customHeight="1">
+      <c r="A71" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30" ht="24" customHeight="1">
+      <c r="A72" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="73" spans="1:30" ht="24" customHeight="1">
+      <c r="B73" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:30" ht="24" customHeight="1">
+      <c r="B74" s="11"/>
+      <c r="AA74" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="AB74" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="AC74" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:30" ht="24" customHeight="1">
+      <c r="A77" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="78" spans="1:30" ht="24" customHeight="1">
+      <c r="B78" s="13" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="80" spans="1:30" ht="24" customHeight="1">
+      <c r="A80" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="81" spans="1:31" ht="24" customHeight="1">
+      <c r="A81" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="82" spans="1:31" ht="24" customHeight="1">
+      <c r="B82" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:31" ht="24" customHeight="1">
+      <c r="A84" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="85" spans="1:31" ht="24" customHeight="1">
+      <c r="A85" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="86" spans="1:31" ht="24" customHeight="1">
+      <c r="B86" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="AA86" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="AB86" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="AC86" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="AD86" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="AE86" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="89" spans="1:31" ht="24" customHeight="1">
+      <c r="A89" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="90" spans="1:31" ht="24" customHeight="1">
+      <c r="B90" s="13" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="92" spans="1:31" ht="24" customHeight="1">
+      <c r="A92" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:31" ht="24" customHeight="1">
+      <c r="A93" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="94" spans="1:31" ht="24" customHeight="1">
+      <c r="B94" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="1:31" ht="24" customHeight="1">
+      <c r="B95" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="AA95" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="AB95" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="AC95" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="AD95" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="AE95" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="97" spans="1:31" ht="24" customHeight="1">
+      <c r="A97" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="98" spans="1:31" ht="24" customHeight="1">
+      <c r="A98" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="99" spans="1:31" ht="24" customHeight="1">
+      <c r="B99" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="1:31" ht="24" customHeight="1">
+      <c r="B100" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="AA100" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="AB100" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="AC100" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD100" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="AE100" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="101" spans="1:31" ht="24" customHeight="1">
+      <c r="B101" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="AA101" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="AB101" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="AC101" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD101" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="AE101" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="103" spans="1:31" ht="24" customHeight="1">
+      <c r="A103" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="104" spans="1:31" ht="24" customHeight="1">
+      <c r="A104" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="105" spans="1:31" ht="24" customHeight="1">
+      <c r="B105" s="11"/>
+      <c r="AA105" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="AB105" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="AC105" s="6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="107" spans="1:31" ht="24" customHeight="1">
+      <c r="A107" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="108" spans="1:31" ht="24" customHeight="1">
+      <c r="A108" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="24" customHeight="1">
-      <c r="B38" s="11"/>
-    </row>
-    <row r="40" spans="1:3" ht="24" customHeight="1">
-      <c r="A40" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="24" customHeight="1">
-      <c r="A41" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="24" customHeight="1">
-      <c r="B42" s="11"/>
-    </row>
-    <row r="45" spans="1:3" ht="24" customHeight="1">
-      <c r="A45" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="24" customHeight="1">
-      <c r="B46" s="13" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="24" customHeight="1">
-      <c r="A48" s="9" t="s">
-        <v>322</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="49" spans="1:31" ht="24" customHeight="1">
-      <c r="A49" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="50" spans="1:31" ht="24" customHeight="1">
-      <c r="B50" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="AA50" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="AB50" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="AC50" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="AD50" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="AE50" s="6" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="52" spans="1:31" ht="24" customHeight="1">
-      <c r="A52" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="53" spans="1:31" ht="24" customHeight="1">
-      <c r="A53" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="54" spans="1:31" ht="24" customHeight="1">
-      <c r="B54" s="10" t="s">
+      <c r="B108" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="109" spans="1:31" ht="24" customHeight="1">
+      <c r="B109" s="11"/>
+    </row>
+    <row r="111" spans="1:31" ht="24" customHeight="1">
+      <c r="A111" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="112" spans="1:31" ht="24" customHeight="1">
+      <c r="A112" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="C112" s="10" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="113" spans="1:30" ht="24" customHeight="1">
+      <c r="B113" s="11"/>
+      <c r="AA113" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="AB113" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="AC113" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="AD113" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="116" spans="1:30" ht="24" customHeight="1">
+      <c r="A116" s="12" t="s">
+        <v>403</v>
+      </c>
+      <c r="B116" s="12" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="117" spans="1:30" ht="24" customHeight="1">
+      <c r="B117" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="119" spans="1:30" ht="24" customHeight="1">
+      <c r="A119" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="120" spans="1:30" ht="24" customHeight="1">
+      <c r="A120" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="121" spans="1:30" ht="24" customHeight="1">
+      <c r="B121" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="24" customHeight="1">
-      <c r="B55" s="11"/>
-      <c r="AA55" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="AB55" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="AC55" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="AD55" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:31" ht="24" customHeight="1">
-      <c r="A57" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="58" spans="1:31" ht="24" customHeight="1">
-      <c r="A58" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B58" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="59" spans="1:31" ht="24" customHeight="1">
-      <c r="B59" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="60" spans="1:31" ht="24" customHeight="1">
-      <c r="B60" s="11"/>
-      <c r="AA60" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="AB60" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="AC60" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="AD60" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:31" ht="24" customHeight="1">
-      <c r="A63" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="64" spans="1:31" ht="24" customHeight="1">
-      <c r="B64" s="13" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="66" spans="1:30" ht="24" customHeight="1">
-      <c r="A66" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="67" spans="1:30" ht="24" customHeight="1">
-      <c r="A67" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="68" spans="1:30" ht="24" customHeight="1">
-      <c r="B68" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="AA68" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="AB68" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="AC68" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="AD68" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="70" spans="1:30" ht="24" customHeight="1">
-      <c r="A70" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="71" spans="1:30" ht="24" customHeight="1">
-      <c r="A71" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="72" spans="1:30" ht="24" customHeight="1">
-      <c r="B72" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="73" spans="1:30" ht="24" customHeight="1">
-      <c r="B73" s="11"/>
-      <c r="AA73" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="AB73" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="AC73" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="76" spans="1:30" ht="24" customHeight="1">
-      <c r="A76" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="77" spans="1:30" ht="24" customHeight="1">
-      <c r="B77" s="13" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="79" spans="1:30" ht="24" customHeight="1">
-      <c r="A79" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="80" spans="1:30" ht="24" customHeight="1">
-      <c r="A80" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>361</v>
-      </c>
-      <c r="C80" s="10" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="81" spans="1:31" ht="24" customHeight="1">
-      <c r="B81" s="11"/>
-    </row>
-    <row r="83" spans="1:31" ht="24" customHeight="1">
-      <c r="A83" s="9" t="s">
-        <v>363</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="84" spans="1:31" ht="24" customHeight="1">
-      <c r="A84" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B84" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="C84" s="10" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="85" spans="1:31" ht="24" customHeight="1">
-      <c r="B85" s="11" t="s">
-        <v>367</v>
-      </c>
-      <c r="AA85" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="AB85" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="AC85" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="AD85" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="AE85" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="88" spans="1:31" ht="24" customHeight="1">
-      <c r="A88" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="B88" s="12" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="89" spans="1:31" ht="24" customHeight="1">
-      <c r="B89" s="13" t="s">
+    <row r="122" spans="1:30" ht="24" customHeight="1">
+      <c r="B122" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="AA122" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="AB122" s="6" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="124" spans="1:30" ht="24" customHeight="1">
+      <c r="A124" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="B124" s="9" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="125" spans="1:30" ht="24" customHeight="1">
+      <c r="A125" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B125" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="C125" s="10" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="126" spans="1:30" ht="24" customHeight="1">
+      <c r="B126" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:30" ht="24" customHeight="1">
+      <c r="A128" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="129" spans="1:28" ht="24" customHeight="1">
+      <c r="A129" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B129" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="C129" s="10" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="130" spans="1:28" ht="24" customHeight="1">
+      <c r="B130" s="11" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="91" spans="1:31" ht="24" customHeight="1">
-      <c r="A91" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="92" spans="1:31" ht="24" customHeight="1">
-      <c r="A92" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B92" s="10" t="s">
-        <v>375</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="93" spans="1:31" ht="24" customHeight="1">
-      <c r="B93" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="94" spans="1:31" ht="24" customHeight="1">
-      <c r="B94" s="11" t="s">
-        <v>377</v>
-      </c>
-      <c r="AA94" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="AB94" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="AC94" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="AD94" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="AE94" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="96" spans="1:31" ht="24" customHeight="1">
-      <c r="A96" s="9" t="s">
-        <v>381</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="97" spans="1:31" ht="24" customHeight="1">
-      <c r="A97" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B97" s="10" t="s">
-        <v>383</v>
-      </c>
-      <c r="C97" s="10" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="98" spans="1:31" ht="24" customHeight="1">
-      <c r="B98" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="99" spans="1:31" ht="24" customHeight="1">
-      <c r="B99" s="11"/>
-      <c r="AA99" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="AB99" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="AC99" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="AD99" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="AE99" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="101" spans="1:31" ht="24" customHeight="1">
-      <c r="A101" s="9" t="s">
-        <v>389</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="102" spans="1:31" ht="24" customHeight="1">
-      <c r="A102" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B102" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="C102" s="10" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="103" spans="1:31" ht="24" customHeight="1">
-      <c r="B103" s="11"/>
-      <c r="AA103" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="AB103" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="AC103" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="105" spans="1:31" ht="24" customHeight="1">
-      <c r="A105" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="B105" s="9" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="106" spans="1:31" ht="24" customHeight="1">
-      <c r="A106" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B106" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="C106" s="10" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="107" spans="1:31" ht="24" customHeight="1">
-      <c r="B107" s="11"/>
-    </row>
-    <row r="109" spans="1:31" ht="24" customHeight="1">
-      <c r="A109" s="9" t="s">
-        <v>400</v>
-      </c>
-      <c r="B109" s="9" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="110" spans="1:31" ht="24" customHeight="1">
-      <c r="A110" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B110" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="C110" s="10" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="111" spans="1:31" ht="24" customHeight="1">
-      <c r="B111" s="11"/>
-      <c r="AA111" s="6" t="s">
-        <v>404</v>
-      </c>
-      <c r="AB111" s="6" t="s">
-        <v>405</v>
-      </c>
-      <c r="AC111" s="6" t="s">
-        <v>406</v>
-      </c>
-      <c r="AD111" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="114" spans="1:28" ht="24" customHeight="1">
-      <c r="A114" s="12" t="s">
-        <v>407</v>
-      </c>
-      <c r="B114" s="12" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="115" spans="1:28" ht="24" customHeight="1">
-      <c r="B115" s="13" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="117" spans="1:28" ht="24" customHeight="1">
-      <c r="A117" s="9" t="s">
-        <v>410</v>
-      </c>
-      <c r="B117" s="9" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="118" spans="1:28" ht="24" customHeight="1">
-      <c r="A118" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B118" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="C118" s="10" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="119" spans="1:28" ht="24" customHeight="1">
-      <c r="B119" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="120" spans="1:28" ht="24" customHeight="1">
-      <c r="B120" s="11"/>
-      <c r="AA120" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="AB120" s="6" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="122" spans="1:28" ht="24" customHeight="1">
-      <c r="A122" s="9" t="s">
-        <v>416</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="123" spans="1:28" ht="24" customHeight="1">
-      <c r="A123" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="B123" s="10" t="s">
-        <v>418</v>
-      </c>
-      <c r="C123" s="10" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="124" spans="1:28" ht="24" customHeight="1">
-      <c r="B124" s="11"/>
-    </row>
-    <row r="126" spans="1:28" ht="24" customHeight="1">
-      <c r="A126" s="9" t="s">
+      <c r="AA130" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="AB130" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="B126" s="9" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="127" spans="1:28" ht="24" customHeight="1">
-      <c r="A127" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B127" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="C127" s="10" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="128" spans="1:28" ht="24" customHeight="1">
-      <c r="B128" s="11"/>
-      <c r="AA128" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="AB128" s="6" t="s">
-        <v>424</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="18">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B126 B82" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51 B20:B21 B95 B86 B100:B101" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>AA20:AE20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
-      <formula1>AA25:AC25</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26 B105 B74 B31" xr:uid="{00000000-0002-0000-0300-000002000000}">
+      <formula1>AA26:AC26</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30">
-      <formula1>AA30:AC30</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56 B113 B69 B61" xr:uid="{00000000-0002-0000-0300-000005000000}">
+      <formula1>AA56:AD56</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B50">
-      <formula1>AA50:AE50</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
-      <formula1>AA55:AD55</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60">
-      <formula1>AA60:AD60</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B68">
-      <formula1>AA68:AD68</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B73">
-      <formula1>AA73:AC73</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B85">
-      <formula1>AA85:AE85</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B94">
-      <formula1>AA94:AE94</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B99">
-      <formula1>AA99:AE99</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B103">
-      <formula1>AA103:AC103</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B111">
-      <formula1>AA111:AD111</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B120">
-      <formula1>AA120:AB120</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B124">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B128">
-      <formula1>AA128:AB128</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B122 B130" xr:uid="{00000000-0002-0000-0300-00000F000000}">
+      <formula1>AA122:AB122</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>